<commit_message>
v2 launch, pilot complete
</commit_message>
<xml_diff>
--- a/Pilot/rootDesignMatrix.xlsx
+++ b/Pilot/rootDesignMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erene\OneDrive\Desktop\PFC Layers\PFC_Layers_ResponseMapping\Pilot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\PFC_Layers\PFC_Layers_ResponseMapping\Pilot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1395C26-E698-4D9E-8774-B93458A41DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA59DECC-E7DA-4D9E-B094-54FEA08563BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="21">
   <si>
     <t>category</t>
   </si>
@@ -47,18 +47,6 @@
     <t>stimfile</t>
   </si>
   <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>auto</t>
-  </si>
-  <si>
-    <t>fist</t>
-  </si>
-  <si>
-    <t>tur</t>
-  </si>
-  <si>
     <t>resp1</t>
   </si>
   <si>
@@ -77,12 +65,6 @@
     <t>resp8</t>
   </si>
   <si>
-    <t>resp9</t>
-  </si>
-  <si>
-    <t>resp0</t>
-  </si>
-  <si>
     <t>taskCue</t>
   </si>
   <si>
@@ -96,6 +78,27 @@
   </si>
   <si>
     <t>stim//ori1.png</t>
+  </si>
+  <si>
+    <t>shoe</t>
+  </si>
+  <si>
+    <t>resp5</t>
+  </si>
+  <si>
+    <t>resp6</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>horse</t>
+  </si>
+  <si>
+    <t>turtle</t>
+  </si>
+  <si>
+    <t>objFirst</t>
   </si>
 </sst>
 </file>
@@ -453,23 +456,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="16381" max="16384" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="16380" max="16384" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,994 +480,997 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D33" si="0">CONCATENATE("stim//",A2,B2,".png")</f>
-        <v>stim//cat1.png</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car1.png</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat1.png</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car1.png</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat2.png</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car2.png</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat2.png</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car2.png</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat3.png</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car3.png</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat3.png</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car3.png</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat4.png</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car4.png</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>stim//cat4.png</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//car4.png</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto1.png</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//horse1.png</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto1.png</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//horse1.png</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto2.png</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//horse2.png</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto2.png</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//horse2.png</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto3.png</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//horse3.png</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto3.png</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>stim//horse3.png</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto4.png</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse4.png</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>stim//auto4.png</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse4.png</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist1.png</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe1.png</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist1.png</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe1.png</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist2.png</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe2.png</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist2.png</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe2.png</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist3.png</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe3.png</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist3.png</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe3.png</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist4.png</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe4.png</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>stim//fist4.png</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe4.png</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur1.png</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle1.png</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur1.png</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle1.png</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur2.png</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle2.png</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur2.png</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle2.png</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur3.png</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle3.png</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur3.png</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle3.png</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur4.png</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle4.png</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>stim//tur4.png</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle4.png</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" ref="D34:D65" si="1">CONCATENATE("stim//",A34,B34,".png")</f>
-        <v>stim//cat1.png</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car1.png</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat1.png</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car1.png</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat2.png</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car2.png</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat2.png</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car2.png</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat3.png</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car3.png</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat3.png</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car3.png</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat4.png</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car4.png</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>stim//cat4.png</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//car4.png</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto1.png</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse1.png</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto1.png</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse1.png</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto2.png</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse2.png</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto2.png</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse2.png</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto3.png</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse3.png</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B47">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto3.png</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse3.png</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B48">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto4.png</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse4.png</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B49">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
-        <v>stim//auto4.png</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//horse4.png</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist1.png</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe1.png</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist1.png</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe1.png</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist2.png</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe2.png</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist2.png</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe2.png</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist3.png</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe3.png</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist3.png</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe3.png</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist4.png</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe4.png</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B57">
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="1"/>
-        <v>stim//fist4.png</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//shoe4.png</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur1.png</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle1.png</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur1.png</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle1.png</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B60">
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur2.png</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle2.png</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur2.png</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle2.png</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur3.png</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle3.png</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur3.png</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle3.png</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B64">
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur4.png</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>stim//turtle4.png</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B65">
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="1"/>
-        <v>stim//tur4.png</v>
+        <v>stim//turtle4.png</v>
       </c>
     </row>
   </sheetData>

</xml_diff>